<commit_message>
Adding more emoji's in the seed data
</commit_message>
<xml_diff>
--- a/Notes/Associations.xlsx
+++ b/Notes/Associations.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
   <si>
     <t>Users</t>
   </si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t>Sting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">story_title </t>
   </si>
   <si>
     <t>user_id</t>
@@ -815,8 +812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -982,7 +979,7 @@
     </row>
     <row r="18" spans="2:7">
       <c r="B18" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" s="21" t="s">
         <v>23</v>
@@ -1006,10 +1003,10 @@
     </row>
     <row r="20" spans="2:7">
       <c r="B20" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>28</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>29</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
@@ -1084,7 +1081,7 @@
     </row>
     <row r="31" spans="2:7">
       <c r="B31" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C31" s="23"/>
       <c r="D31" s="23"/>
@@ -1127,7 +1124,7 @@
         <v>1</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
@@ -1160,7 +1157,7 @@
     </row>
     <row r="39" spans="2:7">
       <c r="B39" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C39" s="23"/>
       <c r="D39" s="23"/>
@@ -1211,12 +1208,8 @@
       <c r="G43" s="4"/>
     </row>
     <row r="44" spans="2:7">
-      <c r="B44" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>23</v>
-      </c>
+      <c r="B44" s="8"/>
+      <c r="C44" s="9"/>
       <c r="D44" s="9"/>
       <c r="E44" s="9"/>
       <c r="F44" s="9"/>

</xml_diff>